<commit_message>
more edits to rosters
</commit_message>
<xml_diff>
--- a/teams-and-rosters/CS320-Sp22-101-roster.xlsx
+++ b/teams-and-rosters/CS320-Sp22-101-roster.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2022-private\Rosters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2022-private\rosters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEEB850-2C25-44B2-A23A-A71349DB3A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A70A44A-9D27-4DB4-8DE9-C883BA1A2835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="588" yWindow="1206" windowWidth="22452" windowHeight="11754" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="894" yWindow="450" windowWidth="22026" windowHeight="11784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CS320-Sp22-101-roster" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>E-Mail</t>
   </si>
   <si>
-    <t>CS320 Section 101 (MWF 8:00 - 8:50)</t>
-  </si>
-  <si>
     <t>Barthelmes</t>
   </si>
   <si>
@@ -191,6 +188,9 @@
   </si>
   <si>
     <t>gabdalla@ycp.edu</t>
+  </si>
+  <si>
+    <t>CS320 Section 101 (M-W-F 8:00 - 8:50)</t>
   </si>
 </sst>
 </file>
@@ -717,10 +717,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1103,7 +1103,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E18"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1116,13 +1116,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="A1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A2" s="4"/>
@@ -1150,257 +1150,257 @@
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="C9" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="C10" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>41</v>
+        <v>31</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="C12" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="C13" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>43</v>
+        <v>31</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="C15" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="C16" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>45</v>
+        <v>31</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="C17" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>46</v>
+        <v>31</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>47</v>
+      <c r="E18" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>